<commit_message>
Updated USA labor data.
</commit_message>
<xml_diff>
--- a/data/Excel Workbooks/UnitedStatesDataWorkbook.xlsx
+++ b/data/Excel Workbooks/UnitedStatesDataWorkbook.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="22905"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="23206"/>
   <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="480" yWindow="320" windowWidth="27140" windowHeight="17240" firstSheet="9" activeTab="10"/>
+    <workbookView xWindow="480" yWindow="320" windowWidth="27140" windowHeight="17240"/>
   </bookViews>
   <sheets>
     <sheet name="United States Workbook" sheetId="1" r:id="rId1"/>
@@ -1167,7 +1167,7 @@
     <numFmt numFmtId="170" formatCode="_(* #,##0.0000_);_(* \(#,##0.0000\);_(* &quot;-&quot;????_);_(@_)"/>
     <numFmt numFmtId="171" formatCode="#,##0.0000"/>
   </numFmts>
-  <fonts count="50" x14ac:knownFonts="1">
+  <fonts count="51" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1527,6 +1527,13 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="48">
@@ -3391,7 +3398,7 @@
     <xf numFmtId="0" fontId="41" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="42" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="153">
+  <cellXfs count="155">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -3705,6 +3712,8 @@
     <xf numFmtId="171" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="47" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -3720,12 +3729,6 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -3738,6 +3741,12 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
@@ -3747,8 +3756,12 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="47" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="3" fontId="8" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="3" fontId="50" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1124">
     <cellStyle name="•\Ž¦Ï‚Ý‚ÌƒnƒCƒp[ƒŠƒ“ƒN" xfId="2"/>
@@ -5583,19 +5596,19 @@
                   <c:v>1.415492804660667</c:v>
                 </c:pt>
                 <c:pt idx="27">
-                  <c:v>1.425323898960915</c:v>
+                  <c:v>1.425242380766054</c:v>
                 </c:pt>
                 <c:pt idx="28">
-                  <c:v>1.409938698317464</c:v>
+                  <c:v>1.410036520151298</c:v>
                 </c:pt>
                 <c:pt idx="29">
-                  <c:v>1.332317073170732</c:v>
+                  <c:v>1.332083387678796</c:v>
                 </c:pt>
                 <c:pt idx="30">
-                  <c:v>1.331762749445676</c:v>
+                  <c:v>1.332143167688361</c:v>
                 </c:pt>
                 <c:pt idx="31">
-                  <c:v>1.374182100778227</c:v>
+                  <c:v>1.35219664362419</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -6276,11 +6289,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="2091445096"/>
-        <c:axId val="2091454376"/>
+        <c:axId val="2141821432"/>
+        <c:axId val="2141977976"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="2091445096"/>
+        <c:axId val="2141821432"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="2015.0"/>
@@ -6304,7 +6317,6 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
@@ -6321,12 +6333,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="2091454376"/>
+        <c:crossAx val="2141977976"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="2091454376"/>
+        <c:axId val="2141977976"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="3.0"/>
@@ -6374,7 +6386,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="2091445096"/>
+        <c:crossAx val="2141821432"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
         <c:majorUnit val="1.0"/>
@@ -6423,7 +6435,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:title>
     <c:autoTitleDeleted val="0"/>
@@ -7318,11 +7329,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="2109936824"/>
-        <c:axId val="2109944840"/>
+        <c:axId val="-2142531656"/>
+        <c:axId val="-2142523640"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="2109936824"/>
+        <c:axId val="-2142531656"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="2011.0"/>
@@ -7346,20 +7357,19 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="in"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2109944840"/>
+        <c:crossAx val="-2142523640"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
         <c:majorUnit val="10.0"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="2109944840"/>
+        <c:axId val="-2142523640"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -7381,21 +7391,19 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="in"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2109936824"/>
+        <c:crossAx val="-2142531656"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
@@ -7440,7 +7448,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:title>
     <c:autoTitleDeleted val="0"/>
@@ -8443,11 +8450,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="2109995128"/>
-        <c:axId val="2110003416"/>
+        <c:axId val="2141585944"/>
+        <c:axId val="2142156152"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="2109995128"/>
+        <c:axId val="2141585944"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="2011.0"/>
@@ -8476,20 +8483,19 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="in"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2110003416"/>
+        <c:crossAx val="2142156152"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
         <c:majorUnit val="10.0"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="2110003416"/>
+        <c:axId val="2142156152"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -8516,21 +8522,19 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="in"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2109995128"/>
+        <c:crossAx val="2141585944"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
@@ -9004,19 +9008,19 @@
                   <c:v>2.20490284998864</c:v>
                 </c:pt>
                 <c:pt idx="27">
-                  <c:v>2.261698935788131</c:v>
+                  <c:v>2.26160846900418</c:v>
                 </c:pt>
                 <c:pt idx="28">
-                  <c:v>2.281854308889451</c:v>
+                  <c:v>2.281966535252733</c:v>
                 </c:pt>
                 <c:pt idx="29">
-                  <c:v>2.216081345704399</c:v>
+                  <c:v>2.21580758103519</c:v>
                 </c:pt>
                 <c:pt idx="30">
-                  <c:v>2.249452135293525</c:v>
+                  <c:v>2.249850579906756</c:v>
                 </c:pt>
                 <c:pt idx="31">
-                  <c:v>2.326758493038608</c:v>
+                  <c:v>2.301680692031975</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -9233,19 +9237,19 @@
                   <c:v>2.205536666361343</c:v>
                 </c:pt>
                 <c:pt idx="27">
-                  <c:v>2.263045948176289</c:v>
+                  <c:v>2.262958231025475</c:v>
                 </c:pt>
                 <c:pt idx="28">
-                  <c:v>2.282561926612299</c:v>
+                  <c:v>2.28267199591517</c:v>
                 </c:pt>
                 <c:pt idx="29">
-                  <c:v>2.216980664556651</c:v>
+                  <c:v>2.216713208018187</c:v>
                 </c:pt>
                 <c:pt idx="30">
-                  <c:v>2.25530149332791</c:v>
+                  <c:v>2.255658246540594</c:v>
                 </c:pt>
                 <c:pt idx="31">
-                  <c:v>2.328915629892147</c:v>
+                  <c:v>2.305181881787522</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -9456,11 +9460,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="2132009112"/>
-        <c:axId val="2132000408"/>
+        <c:axId val="-2142443080"/>
+        <c:axId val="-2142439944"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="2132009112"/>
+        <c:axId val="-2142443080"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -9470,12 +9474,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2132000408"/>
+        <c:crossAx val="-2142439944"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="2132000408"/>
+        <c:axId val="-2142439944"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -9486,7 +9490,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2132009112"/>
+        <c:crossAx val="-2142443080"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -10473,8 +10477,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AG47"/>
   <sheetViews>
-    <sheetView zoomScale="70" zoomScaleNormal="70" zoomScalePageLayoutView="70" workbookViewId="0">
-      <selection activeCell="A6" sqref="A6"/>
+    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" zoomScalePageLayoutView="70" workbookViewId="0">
+      <selection activeCell="C10" sqref="C10:C41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
@@ -10652,75 +10656,75 @@
     </row>
     <row r="8" spans="1:20" ht="15" customHeight="1">
       <c r="A8" s="16"/>
-      <c r="B8" s="137" t="s">
+      <c r="B8" s="139" t="s">
         <v>127</v>
       </c>
-      <c r="C8" s="137" t="s">
+      <c r="C8" s="139" t="s">
         <v>2</v>
       </c>
-      <c r="D8" s="137" t="s">
+      <c r="D8" s="139" t="s">
         <v>128</v>
       </c>
-      <c r="E8" s="137" t="s">
+      <c r="E8" s="139" t="s">
         <v>116</v>
       </c>
-      <c r="F8" s="137" t="s">
+      <c r="F8" s="139" t="s">
         <v>3</v>
       </c>
-      <c r="G8" s="137" t="s">
+      <c r="G8" s="139" t="s">
         <v>4</v>
       </c>
       <c r="H8" s="134"/>
-      <c r="I8" s="137" t="s">
+      <c r="I8" s="139" t="s">
         <v>119</v>
       </c>
-      <c r="J8" s="137" t="s">
+      <c r="J8" s="139" t="s">
         <v>120</v>
       </c>
-      <c r="K8" s="137" t="s">
+      <c r="K8" s="139" t="s">
         <v>121</v>
       </c>
-      <c r="L8" s="137" t="s">
+      <c r="L8" s="139" t="s">
         <v>122</v>
       </c>
-      <c r="M8" s="137" t="s">
+      <c r="M8" s="139" t="s">
         <v>123</v>
       </c>
-      <c r="N8" s="137" t="s">
+      <c r="N8" s="139" t="s">
         <v>124</v>
       </c>
-      <c r="O8" s="138" t="s">
+      <c r="O8" s="140" t="s">
         <v>38</v>
       </c>
-      <c r="P8" s="137"/>
-      <c r="Q8" s="137"/>
-      <c r="R8" s="137"/>
-      <c r="S8" s="137"/>
-      <c r="T8" s="137"/>
+      <c r="P8" s="139"/>
+      <c r="Q8" s="139"/>
+      <c r="R8" s="139"/>
+      <c r="S8" s="139"/>
+      <c r="T8" s="139"/>
     </row>
     <row r="9" spans="1:20">
       <c r="A9" s="20" t="s">
         <v>0</v>
       </c>
-      <c r="B9" s="137"/>
-      <c r="C9" s="137"/>
-      <c r="D9" s="137"/>
-      <c r="E9" s="137"/>
-      <c r="F9" s="137"/>
-      <c r="G9" s="137"/>
+      <c r="B9" s="139"/>
+      <c r="C9" s="139"/>
+      <c r="D9" s="139"/>
+      <c r="E9" s="139"/>
+      <c r="F9" s="139"/>
+      <c r="G9" s="139"/>
       <c r="H9" s="134"/>
-      <c r="I9" s="137"/>
-      <c r="J9" s="137"/>
-      <c r="K9" s="137"/>
-      <c r="L9" s="137"/>
-      <c r="M9" s="137"/>
-      <c r="N9" s="137"/>
-      <c r="O9" s="138"/>
-      <c r="P9" s="137"/>
-      <c r="Q9" s="137"/>
-      <c r="R9" s="137"/>
-      <c r="S9" s="137"/>
-      <c r="T9" s="137"/>
+      <c r="I9" s="139"/>
+      <c r="J9" s="139"/>
+      <c r="K9" s="139"/>
+      <c r="L9" s="139"/>
+      <c r="M9" s="139"/>
+      <c r="N9" s="139"/>
+      <c r="O9" s="140"/>
+      <c r="P9" s="139"/>
+      <c r="Q9" s="139"/>
+      <c r="R9" s="139"/>
+      <c r="S9" s="139"/>
+      <c r="T9" s="139"/>
     </row>
     <row r="10" spans="1:20">
       <c r="A10" s="21">
@@ -10729,7 +10733,7 @@
       <c r="B10" s="25">
         <v>5833975</v>
       </c>
-      <c r="C10" s="8">
+      <c r="C10" s="153">
         <v>184008</v>
       </c>
       <c r="D10" s="25">
@@ -10789,7 +10793,7 @@
       <c r="B11" s="25">
         <v>5982075</v>
       </c>
-      <c r="C11" s="8">
+      <c r="C11" s="153">
         <v>184394</v>
       </c>
       <c r="D11" s="25">
@@ -10849,7 +10853,7 @@
       <c r="B12" s="25">
         <v>5865925</v>
       </c>
-      <c r="C12" s="8">
+      <c r="C12" s="153">
         <v>181648</v>
       </c>
       <c r="D12" s="25">
@@ -10909,7 +10913,7 @@
       <c r="B13" s="25">
         <v>6130925</v>
       </c>
-      <c r="C13" s="8">
+      <c r="C13" s="153">
         <v>184908</v>
       </c>
       <c r="D13" s="25">
@@ -10969,7 +10973,7 @@
       <c r="B14" s="25">
         <v>6571525</v>
       </c>
-      <c r="C14" s="8">
+      <c r="C14" s="153">
         <v>194236</v>
       </c>
       <c r="D14" s="25">
@@ -11029,7 +11033,7 @@
       <c r="B15" s="25">
         <v>6843400</v>
       </c>
-      <c r="C15" s="8">
+      <c r="C15" s="153">
         <v>198678</v>
       </c>
       <c r="D15" s="25">
@@ -11089,7 +11093,7 @@
       <c r="B16" s="25">
         <v>7080500</v>
       </c>
-      <c r="C16" s="8">
+      <c r="C16" s="153">
         <v>201005</v>
       </c>
       <c r="D16" s="25">
@@ -11149,7 +11153,7 @@
       <c r="B17" s="25">
         <v>7307050</v>
       </c>
-      <c r="C17" s="8">
+      <c r="C17" s="153">
         <v>206453</v>
       </c>
       <c r="D17" s="25">
@@ -11209,7 +11213,7 @@
       <c r="B18" s="25">
         <v>7607400</v>
       </c>
-      <c r="C18" s="8">
+      <c r="C18" s="153">
         <v>212615</v>
       </c>
       <c r="D18" s="25">
@@ -11269,7 +11273,7 @@
       <c r="B19" s="25">
         <v>7879175</v>
       </c>
-      <c r="C19" s="8">
+      <c r="C19" s="153">
         <v>218492</v>
       </c>
       <c r="D19" s="25">
@@ -11329,7 +11333,7 @@
       <c r="B20" s="25">
         <v>8027025</v>
       </c>
-      <c r="C20" s="8">
+      <c r="C20" s="153">
         <v>218868</v>
       </c>
       <c r="D20" s="25">
@@ -11389,7 +11393,7 @@
       <c r="B21" s="25">
         <v>8008325</v>
       </c>
-      <c r="C21" s="8">
+      <c r="C21" s="153">
         <v>215771</v>
       </c>
       <c r="D21" s="25">
@@ -11449,7 +11453,7 @@
       <c r="B22" s="25">
         <v>8280025</v>
       </c>
-      <c r="C22" s="8">
+      <c r="C22" s="153">
         <v>215945</v>
       </c>
       <c r="D22" s="25">
@@ -11506,7 +11510,7 @@
       <c r="B23" s="25">
         <v>8516175</v>
       </c>
-      <c r="C23" s="8">
+      <c r="C23" s="153">
         <v>221000</v>
       </c>
       <c r="D23" s="25">
@@ -11563,7 +11567,7 @@
       <c r="B24" s="25">
         <v>8863125</v>
       </c>
-      <c r="C24" s="8">
+      <c r="C24" s="153">
         <v>227916</v>
       </c>
       <c r="D24" s="25">
@@ -11620,7 +11624,7 @@
       <c r="B25" s="25">
         <v>9085975</v>
       </c>
-      <c r="C25" s="8">
+      <c r="C25" s="153">
         <v>233531</v>
       </c>
       <c r="D25" s="25">
@@ -11677,7 +11681,7 @@
       <c r="B26" s="25">
         <v>9425850</v>
       </c>
-      <c r="C26" s="8">
+      <c r="C26" s="153">
         <v>236446</v>
       </c>
       <c r="D26" s="25">
@@ -11734,7 +11738,7 @@
       <c r="B27" s="25">
         <v>9845925</v>
       </c>
-      <c r="C27" s="8">
+      <c r="C27" s="153">
         <v>243372</v>
       </c>
       <c r="D27" s="25">
@@ -11791,7 +11795,7 @@
       <c r="B28" s="25">
         <v>10274750</v>
       </c>
-      <c r="C28" s="8">
+      <c r="C28" s="153">
         <v>248610</v>
       </c>
       <c r="D28" s="25">
@@ -11848,7 +11852,7 @@
       <c r="B29" s="25">
         <v>10770625</v>
       </c>
-      <c r="C29" s="8">
+      <c r="C29" s="153">
         <v>253474</v>
       </c>
       <c r="D29" s="25">
@@ -11905,8 +11909,8 @@
       <c r="B30" s="25">
         <v>11216425</v>
       </c>
-      <c r="C30" s="8">
-        <v>256851.99999999997</v>
+      <c r="C30" s="153">
+        <v>256852</v>
       </c>
       <c r="D30" s="25">
         <v>15409247</v>
@@ -11930,7 +11934,7 @@
       </c>
       <c r="J30" s="15">
         <f t="shared" si="3"/>
-        <v>1.3958740924307638</v>
+        <v>1.395874092430764</v>
       </c>
       <c r="K30" s="15">
         <f t="shared" si="4"/>
@@ -11962,7 +11966,7 @@
       <c r="B31" s="25">
         <v>11337475</v>
       </c>
-      <c r="C31" s="14">
+      <c r="C31" s="154">
         <v>253714</v>
       </c>
       <c r="D31" s="25">
@@ -12016,7 +12020,7 @@
       <c r="B32" s="25">
         <v>11543100</v>
       </c>
-      <c r="C32" s="14">
+      <c r="C32" s="154">
         <v>250412</v>
       </c>
       <c r="D32" s="25">
@@ -12070,7 +12074,7 @@
       <c r="B33" s="25">
         <v>11836425</v>
       </c>
-      <c r="C33" s="14">
+      <c r="C33" s="154">
         <v>249114</v>
       </c>
       <c r="D33" s="25">
@@ -12124,7 +12128,7 @@
       <c r="B34" s="25">
         <v>12246925</v>
       </c>
-      <c r="C34" s="14">
+      <c r="C34" s="154">
         <v>251911</v>
       </c>
       <c r="D34" s="25">
@@ -12178,7 +12182,7 @@
       <c r="B35" s="25">
         <v>12622950</v>
       </c>
-      <c r="C35" s="14">
+      <c r="C35" s="154">
         <v>255787</v>
       </c>
       <c r="D35" s="25">
@@ -12232,7 +12236,7 @@
       <c r="B36" s="25">
         <v>12958475</v>
       </c>
-      <c r="C36" s="14">
+      <c r="C36" s="154">
         <v>260462</v>
       </c>
       <c r="D36" s="25">
@@ -12286,8 +12290,8 @@
       <c r="B37" s="25">
         <v>13206375</v>
       </c>
-      <c r="C37" s="14">
-        <v>262271</v>
+      <c r="C37" s="154">
+        <v>262256</v>
       </c>
       <c r="D37" s="25">
         <v>20705340</v>
@@ -12309,7 +12313,7 @@
       </c>
       <c r="J37" s="15">
         <f t="shared" si="3"/>
-        <v>1.4253238989609147</v>
+        <v>1.4252423807660537</v>
       </c>
       <c r="K37" s="15">
         <f t="shared" si="4"/>
@@ -12340,8 +12344,8 @@
       <c r="B38" s="25">
         <v>13161925</v>
       </c>
-      <c r="C38" s="14">
-        <v>259440</v>
+      <c r="C38" s="154">
+        <v>259458</v>
       </c>
       <c r="D38" s="25">
         <v>21234566</v>
@@ -12363,7 +12367,7 @@
       </c>
       <c r="J38" s="15">
         <f t="shared" si="3"/>
-        <v>1.4099386983174644</v>
+        <v>1.4100365201512979</v>
       </c>
       <c r="K38" s="15">
         <f t="shared" si="4"/>
@@ -12394,8 +12398,8 @@
       <c r="B39" s="25">
         <v>12703125</v>
       </c>
-      <c r="C39" s="14">
-        <v>245157</v>
+      <c r="C39" s="154">
+        <v>245114</v>
       </c>
       <c r="D39" s="25">
         <v>21354496</v>
@@ -12417,7 +12421,7 @@
       </c>
       <c r="J39" s="15">
         <f t="shared" si="3"/>
-        <v>1.3323170731707317</v>
+        <v>1.3320833876787965</v>
       </c>
       <c r="K39" s="15">
         <f t="shared" si="4"/>
@@ -12448,8 +12452,8 @@
       <c r="B40" s="25">
         <v>13087975</v>
       </c>
-      <c r="C40" s="14">
-        <v>245055</v>
+      <c r="C40" s="154">
+        <v>245125</v>
       </c>
       <c r="D40" s="25">
         <v>21508031</v>
@@ -12471,7 +12475,7 @@
       </c>
       <c r="J40" s="15">
         <f t="shared" si="3"/>
-        <v>1.3317627494456763</v>
+        <v>1.3321431676883613</v>
       </c>
       <c r="K40" s="15">
         <f t="shared" si="4"/>
@@ -12502,8 +12506,8 @@
       <c r="B41" s="25">
         <v>13315075</v>
       </c>
-      <c r="C41" s="14">
-        <v>252860.5</v>
+      <c r="C41" s="154">
+        <v>248815</v>
       </c>
       <c r="D41" s="25">
         <v>21763469</v>
@@ -12525,7 +12529,7 @@
       </c>
       <c r="J41" s="15">
         <f t="shared" si="3"/>
-        <v>1.3741821007782271</v>
+        <v>1.3521966436241903</v>
       </c>
       <c r="K41" s="15">
         <f t="shared" si="4"/>
@@ -12619,12 +12623,6 @@
     </row>
   </sheetData>
   <mergeCells count="18">
-    <mergeCell ref="C8:C9"/>
-    <mergeCell ref="F8:F9"/>
-    <mergeCell ref="G8:G9"/>
-    <mergeCell ref="E8:E9"/>
-    <mergeCell ref="B8:B9"/>
-    <mergeCell ref="D8:D9"/>
     <mergeCell ref="T8:T9"/>
     <mergeCell ref="I8:I9"/>
     <mergeCell ref="J8:J9"/>
@@ -12637,6 +12635,12 @@
     <mergeCell ref="S8:S9"/>
     <mergeCell ref="O8:O9"/>
     <mergeCell ref="L8:L9"/>
+    <mergeCell ref="C8:C9"/>
+    <mergeCell ref="F8:F9"/>
+    <mergeCell ref="G8:G9"/>
+    <mergeCell ref="E8:E9"/>
+    <mergeCell ref="B8:B9"/>
+    <mergeCell ref="D8:D9"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait"/>
@@ -13453,7 +13457,7 @@
       </c>
       <c r="D22" s="136">
         <f>'United States Workbook'!J30</f>
-        <v>1.3958740924307638</v>
+        <v>1.395874092430764</v>
       </c>
       <c r="E22" s="136">
         <f>'United States Workbook'!K30</f>
@@ -13712,7 +13716,7 @@
       </c>
       <c r="D29" s="136">
         <f>'United States Workbook'!J37</f>
-        <v>1.4253238989609147</v>
+        <v>1.4252423807660537</v>
       </c>
       <c r="E29" s="136">
         <f>'United States Workbook'!K37</f>
@@ -13749,7 +13753,7 @@
       </c>
       <c r="D30" s="136">
         <f>'United States Workbook'!J38</f>
-        <v>1.4099386983174644</v>
+        <v>1.4100365201512979</v>
       </c>
       <c r="E30" s="136">
         <f>'United States Workbook'!K38</f>
@@ -13786,7 +13790,7 @@
       </c>
       <c r="D31" s="136">
         <f>'United States Workbook'!J39</f>
-        <v>1.3323170731707317</v>
+        <v>1.3320833876787965</v>
       </c>
       <c r="E31" s="136">
         <f>'United States Workbook'!K39</f>
@@ -13823,7 +13827,7 @@
       </c>
       <c r="D32" s="136">
         <f>'United States Workbook'!J40</f>
-        <v>1.3317627494456763</v>
+        <v>1.3321431676883613</v>
       </c>
       <c r="E32" s="136">
         <f>'United States Workbook'!K40</f>
@@ -13860,7 +13864,7 @@
       </c>
       <c r="D33" s="136">
         <f>'United States Workbook'!J41</f>
-        <v>1.3741821007782271</v>
+        <v>1.3521966436241903</v>
       </c>
       <c r="E33" s="136">
         <f>'United States Workbook'!K41</f>
@@ -13922,24 +13926,24 @@
       <c r="A3" s="3"/>
     </row>
     <row r="4" spans="1:4" s="9" customFormat="1">
-      <c r="A4" s="139" t="s">
+      <c r="A4" s="141" t="s">
         <v>0</v>
       </c>
-      <c r="B4" s="139" t="s">
+      <c r="B4" s="141" t="s">
         <v>41</v>
       </c>
-      <c r="C4" s="139" t="s">
+      <c r="C4" s="141" t="s">
         <v>42</v>
       </c>
-      <c r="D4" s="139" t="s">
+      <c r="D4" s="141" t="s">
         <v>43</v>
       </c>
     </row>
     <row r="5" spans="1:4">
-      <c r="A5" s="139"/>
-      <c r="B5" s="139"/>
-      <c r="C5" s="139"/>
-      <c r="D5" s="139"/>
+      <c r="A5" s="141"/>
+      <c r="B5" s="141"/>
+      <c r="C5" s="141"/>
+      <c r="D5" s="141"/>
     </row>
     <row r="6" spans="1:4">
       <c r="A6" s="39">
@@ -15027,34 +15031,34 @@
       <c r="A28" s="144" t="s">
         <v>0</v>
       </c>
-      <c r="B28" s="140" t="s">
+      <c r="B28" s="142" t="s">
         <v>63</v>
       </c>
       <c r="C28" s="146" t="s">
         <v>30</v>
       </c>
-      <c r="D28" s="140" t="s">
+      <c r="D28" s="142" t="s">
         <v>31</v>
       </c>
-      <c r="E28" s="140" t="s">
+      <c r="E28" s="142" t="s">
         <v>52</v>
       </c>
-      <c r="F28" s="140" t="s">
+      <c r="F28" s="142" t="s">
         <v>54</v>
       </c>
-      <c r="G28" s="140" t="s">
+      <c r="G28" s="142" t="s">
         <v>46</v>
       </c>
-      <c r="H28" s="140" t="s">
+      <c r="H28" s="142" t="s">
         <v>65</v>
       </c>
-      <c r="I28" s="140" t="s">
+      <c r="I28" s="142" t="s">
         <v>66</v>
       </c>
-      <c r="J28" s="140" t="s">
+      <c r="J28" s="142" t="s">
         <v>74</v>
       </c>
-      <c r="K28" s="140" t="s">
+      <c r="K28" s="142" t="s">
         <v>75</v>
       </c>
       <c r="L28" s="144" t="s">
@@ -15063,10 +15067,10 @@
       <c r="M28" s="146" t="s">
         <v>49</v>
       </c>
-      <c r="N28" s="140" t="s">
+      <c r="N28" s="142" t="s">
         <v>51</v>
       </c>
-      <c r="O28" s="140" t="s">
+      <c r="O28" s="142" t="s">
         <v>95</v>
       </c>
       <c r="P28" s="144" t="s">
@@ -15075,25 +15079,25 @@
       <c r="Q28" s="146" t="s">
         <v>33</v>
       </c>
-      <c r="R28" s="140" t="s">
+      <c r="R28" s="142" t="s">
         <v>34</v>
       </c>
-      <c r="S28" s="140" t="s">
+      <c r="S28" s="142" t="s">
         <v>35</v>
       </c>
-      <c r="T28" s="140" t="s">
+      <c r="T28" s="142" t="s">
         <v>36</v>
       </c>
-      <c r="U28" s="140" t="s">
+      <c r="U28" s="142" t="s">
         <v>47</v>
       </c>
-      <c r="V28" s="140" t="s">
+      <c r="V28" s="142" t="s">
         <v>71</v>
       </c>
-      <c r="W28" s="140" t="s">
+      <c r="W28" s="142" t="s">
         <v>73</v>
       </c>
-      <c r="X28" s="142" t="s">
+      <c r="X28" s="148" t="s">
         <v>37</v>
       </c>
       <c r="Y28" s="144" t="s">
@@ -15102,63 +15106,63 @@
       <c r="Z28" s="146" t="s">
         <v>87</v>
       </c>
-      <c r="AA28" s="140" t="s">
+      <c r="AA28" s="142" t="s">
         <v>88</v>
       </c>
-      <c r="AB28" s="140" t="s">
+      <c r="AB28" s="142" t="s">
         <v>89</v>
       </c>
-      <c r="AC28" s="140" t="s">
+      <c r="AC28" s="142" t="s">
         <v>90</v>
       </c>
-      <c r="AD28" s="140" t="s">
+      <c r="AD28" s="142" t="s">
         <v>91</v>
       </c>
-      <c r="AE28" s="140" t="s">
+      <c r="AE28" s="142" t="s">
         <v>92</v>
       </c>
-      <c r="AF28" s="140" t="s">
+      <c r="AF28" s="142" t="s">
         <v>93</v>
       </c>
-      <c r="AG28" s="142" t="s">
+      <c r="AG28" s="148" t="s">
         <v>94</v>
       </c>
       <c r="AI28" s="63"/>
     </row>
     <row r="29" spans="1:35">
       <c r="A29" s="145"/>
-      <c r="B29" s="141"/>
+      <c r="B29" s="143"/>
       <c r="C29" s="147"/>
-      <c r="D29" s="141"/>
-      <c r="E29" s="141"/>
-      <c r="F29" s="141"/>
-      <c r="G29" s="141"/>
-      <c r="H29" s="141"/>
-      <c r="I29" s="141"/>
-      <c r="J29" s="141"/>
-      <c r="K29" s="141"/>
+      <c r="D29" s="143"/>
+      <c r="E29" s="143"/>
+      <c r="F29" s="143"/>
+      <c r="G29" s="143"/>
+      <c r="H29" s="143"/>
+      <c r="I29" s="143"/>
+      <c r="J29" s="143"/>
+      <c r="K29" s="143"/>
       <c r="L29" s="145"/>
       <c r="M29" s="147"/>
-      <c r="N29" s="141"/>
-      <c r="O29" s="141"/>
+      <c r="N29" s="143"/>
+      <c r="O29" s="143"/>
       <c r="P29" s="145"/>
       <c r="Q29" s="147"/>
-      <c r="R29" s="141"/>
-      <c r="S29" s="141"/>
-      <c r="T29" s="141"/>
-      <c r="U29" s="141"/>
-      <c r="V29" s="141"/>
-      <c r="W29" s="141"/>
-      <c r="X29" s="143"/>
+      <c r="R29" s="143"/>
+      <c r="S29" s="143"/>
+      <c r="T29" s="143"/>
+      <c r="U29" s="143"/>
+      <c r="V29" s="143"/>
+      <c r="W29" s="143"/>
+      <c r="X29" s="149"/>
       <c r="Y29" s="145"/>
       <c r="Z29" s="147"/>
-      <c r="AA29" s="141"/>
-      <c r="AB29" s="141"/>
-      <c r="AC29" s="141"/>
-      <c r="AD29" s="141"/>
-      <c r="AE29" s="141"/>
-      <c r="AF29" s="141"/>
-      <c r="AG29" s="143"/>
+      <c r="AA29" s="143"/>
+      <c r="AB29" s="143"/>
+      <c r="AC29" s="143"/>
+      <c r="AD29" s="143"/>
+      <c r="AE29" s="143"/>
+      <c r="AF29" s="143"/>
+      <c r="AG29" s="149"/>
       <c r="AI29" s="112"/>
     </row>
     <row r="30" spans="1:35">
@@ -19463,6 +19467,24 @@
     </row>
   </sheetData>
   <mergeCells count="33">
+    <mergeCell ref="AF28:AF29"/>
+    <mergeCell ref="AG28:AG29"/>
+    <mergeCell ref="AA28:AA29"/>
+    <mergeCell ref="AB28:AB29"/>
+    <mergeCell ref="AC28:AC29"/>
+    <mergeCell ref="AD28:AD29"/>
+    <mergeCell ref="AE28:AE29"/>
+    <mergeCell ref="Y28:Y29"/>
+    <mergeCell ref="Z28:Z29"/>
+    <mergeCell ref="W28:W29"/>
+    <mergeCell ref="S28:S29"/>
+    <mergeCell ref="T28:T29"/>
+    <mergeCell ref="X28:X29"/>
+    <mergeCell ref="A28:A29"/>
+    <mergeCell ref="B28:B29"/>
+    <mergeCell ref="C28:C29"/>
+    <mergeCell ref="D28:D29"/>
+    <mergeCell ref="E28:E29"/>
     <mergeCell ref="F28:F29"/>
     <mergeCell ref="G28:G29"/>
     <mergeCell ref="H28:H29"/>
@@ -19478,24 +19500,6 @@
     <mergeCell ref="I28:I29"/>
     <mergeCell ref="J28:J29"/>
     <mergeCell ref="K28:K29"/>
-    <mergeCell ref="A28:A29"/>
-    <mergeCell ref="B28:B29"/>
-    <mergeCell ref="C28:C29"/>
-    <mergeCell ref="D28:D29"/>
-    <mergeCell ref="E28:E29"/>
-    <mergeCell ref="Y28:Y29"/>
-    <mergeCell ref="Z28:Z29"/>
-    <mergeCell ref="W28:W29"/>
-    <mergeCell ref="S28:S29"/>
-    <mergeCell ref="T28:T29"/>
-    <mergeCell ref="X28:X29"/>
-    <mergeCell ref="AF28:AF29"/>
-    <mergeCell ref="AG28:AG29"/>
-    <mergeCell ref="AA28:AA29"/>
-    <mergeCell ref="AB28:AB29"/>
-    <mergeCell ref="AC28:AC29"/>
-    <mergeCell ref="AD28:AD29"/>
-    <mergeCell ref="AE28:AE29"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <extLst>
@@ -25697,55 +25701,55 @@
     </row>
     <row r="3" spans="1:7">
       <c r="A3" s="16"/>
-      <c r="B3" s="149" t="s">
+      <c r="B3" s="151" t="s">
         <v>7</v>
       </c>
-      <c r="C3" s="149" t="s">
+      <c r="C3" s="151" t="s">
         <v>8</v>
       </c>
-      <c r="D3" s="149" t="s">
+      <c r="D3" s="151" t="s">
         <v>9</v>
       </c>
-      <c r="E3" s="149"/>
-      <c r="F3" s="149"/>
+      <c r="E3" s="151"/>
+      <c r="F3" s="151"/>
       <c r="G3" s="16"/>
     </row>
     <row r="4" spans="1:7">
       <c r="A4" s="16"/>
-      <c r="B4" s="149"/>
-      <c r="C4" s="149"/>
-      <c r="D4" s="149"/>
-      <c r="E4" s="149"/>
-      <c r="F4" s="149"/>
+      <c r="B4" s="151"/>
+      <c r="C4" s="151"/>
+      <c r="D4" s="151"/>
+      <c r="E4" s="151"/>
+      <c r="F4" s="151"/>
       <c r="G4" s="16"/>
     </row>
     <row r="5" spans="1:7" ht="15" customHeight="1">
       <c r="A5" s="16"/>
-      <c r="B5" s="148" t="s">
+      <c r="B5" s="150" t="s">
         <v>6</v>
       </c>
-      <c r="C5" s="148" t="s">
+      <c r="C5" s="150" t="s">
         <v>128</v>
       </c>
-      <c r="D5" s="148" t="s">
+      <c r="D5" s="150" t="s">
         <v>10</v>
       </c>
-      <c r="E5" s="148" t="s">
+      <c r="E5" s="150" t="s">
         <v>11</v>
       </c>
-      <c r="F5" s="148"/>
-      <c r="G5" s="148"/>
+      <c r="F5" s="150"/>
+      <c r="G5" s="150"/>
     </row>
     <row r="6" spans="1:7" ht="27" customHeight="1">
       <c r="A6" s="20" t="s">
         <v>0</v>
       </c>
-      <c r="B6" s="148"/>
-      <c r="C6" s="148"/>
-      <c r="D6" s="148"/>
-      <c r="E6" s="148"/>
-      <c r="F6" s="148"/>
-      <c r="G6" s="149"/>
+      <c r="B6" s="150"/>
+      <c r="C6" s="150"/>
+      <c r="D6" s="150"/>
+      <c r="E6" s="150"/>
+      <c r="F6" s="150"/>
+      <c r="G6" s="151"/>
     </row>
     <row r="7" spans="1:7">
       <c r="A7" s="16">
@@ -27611,23 +27615,23 @@
     </row>
     <row r="3" spans="1:61">
       <c r="A3" s="16"/>
-      <c r="B3" s="149" t="s">
+      <c r="B3" s="151" t="s">
         <v>7</v>
       </c>
-      <c r="C3" s="150" t="s">
+      <c r="C3" s="152" t="s">
         <v>12</v>
       </c>
-      <c r="D3" s="149" t="s">
+      <c r="D3" s="151" t="s">
         <v>9</v>
       </c>
-      <c r="E3" s="149"/>
+      <c r="E3" s="151"/>
     </row>
     <row r="4" spans="1:61" ht="16.5" customHeight="1">
       <c r="A4" s="16"/>
-      <c r="B4" s="149"/>
-      <c r="C4" s="150"/>
-      <c r="D4" s="149"/>
-      <c r="E4" s="149"/>
+      <c r="B4" s="151"/>
+      <c r="C4" s="152"/>
+      <c r="D4" s="151"/>
+      <c r="E4" s="151"/>
       <c r="I4" s="9"/>
       <c r="J4" s="12"/>
       <c r="K4" s="12"/>
@@ -27684,16 +27688,16 @@
     </row>
     <row r="5" spans="1:61" ht="15" customHeight="1">
       <c r="A5" s="16"/>
-      <c r="B5" s="148" t="s">
+      <c r="B5" s="150" t="s">
         <v>1</v>
       </c>
-      <c r="C5" s="148" t="s">
+      <c r="C5" s="150" t="s">
         <v>127</v>
       </c>
-      <c r="D5" s="148" t="s">
+      <c r="D5" s="150" t="s">
         <v>10</v>
       </c>
-      <c r="E5" s="148" t="s">
+      <c r="E5" s="150" t="s">
         <v>11</v>
       </c>
     </row>
@@ -27701,10 +27705,10 @@
       <c r="A6" s="20" t="s">
         <v>0</v>
       </c>
-      <c r="B6" s="148"/>
-      <c r="C6" s="148"/>
-      <c r="D6" s="148"/>
-      <c r="E6" s="148"/>
+      <c r="B6" s="150"/>
+      <c r="C6" s="150"/>
+      <c r="D6" s="150"/>
+      <c r="E6" s="150"/>
       <c r="I6" s="9"/>
       <c r="J6" s="9"/>
       <c r="K6" s="9"/>
@@ -29594,7 +29598,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:R42"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection sqref="A1:R44"/>
     </sheetView>
   </sheetViews>
@@ -29640,14 +29644,14 @@
       <c r="J1" t="s">
         <v>145</v>
       </c>
-      <c r="K1" s="151">
+      <c r="K1" s="137">
         <v>-2.5000000000000001E-2</v>
       </c>
-      <c r="L1" s="152"/>
-      <c r="M1" s="152" t="s">
+      <c r="L1" s="138"/>
+      <c r="M1" s="138" t="s">
         <v>157</v>
       </c>
-      <c r="N1" s="152" t="s">
+      <c r="N1" s="138" t="s">
         <v>158</v>
       </c>
       <c r="O1" t="s">
@@ -29699,32 +29703,32 @@
       <c r="J2" t="s">
         <v>144</v>
       </c>
-      <c r="K2" s="151">
+      <c r="K2" s="137">
         <v>7.0000000000000001E-3</v>
       </c>
-      <c r="L2" s="152"/>
-      <c r="M2" s="152">
-        <f>EXP(lambda_L*B2)</f>
+      <c r="L2" s="138"/>
+      <c r="M2" s="138">
+        <f t="shared" ref="M2:M33" si="0">EXP(lambda_L*B2)</f>
         <v>1</v>
       </c>
-      <c r="N2" s="152">
-        <f>EXP(lambda_E*B2)</f>
+      <c r="N2" s="138">
+        <f t="shared" ref="N2:N33" si="1">EXP(lambda_E*B2)</f>
         <v>1</v>
       </c>
       <c r="O2">
-        <f>E2^alpha * (M2*D2)^beta</f>
+        <f t="shared" ref="O2:O33" si="2">E2^alpha * (M2*D2)^beta</f>
         <v>1</v>
       </c>
       <c r="P2">
-        <f>((1-gamma_E)^1 * O2^phi + gamma_E^1 * ($N2*F2)^phi)^invPhi</f>
+        <f t="shared" ref="P2:P22" si="3">((1-gamma_E)^1 * O2^phi + gamma_E^1 * ($N2*F2)^phi)^invPhi</f>
         <v>1</v>
       </c>
       <c r="Q2" s="123">
-        <f>((1-gamma_E)^1 * P2^phi + gamma_E^1 * ($N2*G2)^phi)^invPhi</f>
+        <f t="shared" ref="Q2:Q22" si="4">((1-gamma_E)^1 * P2^phi + gamma_E^1 * ($N2*G2)^phi)^invPhi</f>
         <v>1</v>
       </c>
       <c r="R2" s="123">
-        <f>((1-gamma_E)^1 * Q2^phi + gamma_E^1 * ($N2*H2)^phi)^invPhi</f>
+        <f t="shared" ref="R2:R22" si="5">((1-gamma_E)^1 * Q2^phi + gamma_E^1 * ($N2*H2)^phi)^invPhi</f>
         <v>1</v>
       </c>
     </row>
@@ -29764,32 +29768,32 @@
       <c r="J3" t="s">
         <v>146</v>
       </c>
-      <c r="K3" s="151">
+      <c r="K3" s="137">
         <v>0.72599999999999998</v>
       </c>
-      <c r="L3" s="152"/>
-      <c r="M3" s="152">
-        <f>EXP(lambda_L*B3)</f>
+      <c r="L3" s="138"/>
+      <c r="M3" s="138">
+        <f t="shared" si="0"/>
         <v>1.0140984589384923</v>
       </c>
-      <c r="N3" s="152">
-        <f>EXP(lambda_E*B3)</f>
+      <c r="N3" s="138">
+        <f t="shared" si="1"/>
         <v>1.0217327903373821</v>
       </c>
       <c r="O3" s="123">
-        <f>E3^alpha * (M3*D3)^beta</f>
+        <f t="shared" si="2"/>
         <v>1.0205785007443666</v>
       </c>
       <c r="P3" s="123">
-        <f>((1-gamma_E)^1 * O3^phi + gamma_E^1 * ($N3*F3)^phi)^invPhi</f>
+        <f t="shared" si="3"/>
         <v>1.0204736215500438</v>
       </c>
       <c r="Q3" s="123">
-        <f>((1-gamma_E)^1 * P3^phi + gamma_E^1 * ($N3*G3)^phi)^invPhi</f>
+        <f t="shared" si="4"/>
         <v>1.0203680908554074</v>
       </c>
       <c r="R3" s="123">
-        <f>((1-gamma_E)^1 * Q3^phi + gamma_E^1 * ($N3*H3)^phi)^invPhi</f>
+        <f t="shared" si="5"/>
         <v>1.0202306018014293</v>
       </c>
     </row>
@@ -29829,32 +29833,32 @@
       <c r="J4" t="s">
         <v>147</v>
       </c>
-      <c r="K4" s="151">
+      <c r="K4" s="137">
         <v>1.4E-2</v>
       </c>
-      <c r="L4" s="152"/>
-      <c r="M4" s="152">
-        <f>EXP(lambda_L*B4)</f>
+      <c r="L4" s="138"/>
+      <c r="M4" s="138">
+        <f t="shared" si="0"/>
         <v>1.028395684421425</v>
       </c>
-      <c r="N4" s="152">
-        <f>EXP(lambda_E*B4)</f>
+      <c r="N4" s="138">
+        <f t="shared" si="1"/>
         <v>1.0439378948506126</v>
       </c>
       <c r="O4" s="123">
-        <f>E4^alpha * (M4*D4)^beta</f>
+        <f t="shared" si="2"/>
         <v>1.0259882977800701</v>
       </c>
       <c r="P4" s="123">
-        <f>((1-gamma_E)^1 * O4^phi + gamma_E^1 * ($N4*F4)^phi)^invPhi</f>
+        <f t="shared" si="3"/>
         <v>1.0258396382572177</v>
       </c>
       <c r="Q4" s="123">
-        <f>((1-gamma_E)^1 * P4^phi + gamma_E^1 * ($N4*G4)^phi)^invPhi</f>
+        <f t="shared" si="4"/>
         <v>1.0256899820668377</v>
       </c>
       <c r="R4" s="123">
-        <f>((1-gamma_E)^1 * Q4^phi + gamma_E^1 * ($N4*H4)^phi)^invPhi</f>
+        <f t="shared" si="5"/>
         <v>1.0255237079030171</v>
       </c>
     </row>
@@ -29894,32 +29898,32 @@
       <c r="J5" t="s">
         <v>148</v>
       </c>
-      <c r="K5" s="151">
+      <c r="K5" s="137">
         <v>2.1499999999999998E-2</v>
       </c>
-      <c r="L5" s="152"/>
-      <c r="M5" s="152">
-        <f>EXP(lambda_L*B5)</f>
+      <c r="L5" s="138"/>
+      <c r="M5" s="138">
+        <f t="shared" si="0"/>
         <v>1.0428944787507632</v>
       </c>
-      <c r="N5" s="152">
-        <f>EXP(lambda_E*B5)</f>
+      <c r="N5" s="138">
+        <f t="shared" si="1"/>
         <v>1.066625578244649</v>
       </c>
       <c r="O5" s="123">
-        <f>E5^alpha * (M5*D5)^beta</f>
+        <f t="shared" si="2"/>
         <v>1.057454399273293</v>
       </c>
       <c r="P5" s="123">
-        <f>((1-gamma_E)^1 * O5^phi + gamma_E^1 * ($N5*F5)^phi)^invPhi</f>
+        <f t="shared" si="3"/>
         <v>1.0572887745364343</v>
       </c>
       <c r="Q5" s="123">
-        <f>((1-gamma_E)^1 * P5^phi + gamma_E^1 * ($N5*G5)^phi)^invPhi</f>
+        <f t="shared" si="4"/>
         <v>1.0571226163790735</v>
       </c>
       <c r="R5" s="123">
-        <f>((1-gamma_E)^1 * Q5^phi + gamma_E^1 * ($N5*H5)^phi)^invPhi</f>
+        <f t="shared" si="5"/>
         <v>1.0569474056228705</v>
       </c>
     </row>
@@ -29966,28 +29970,28 @@
       <c r="L6" s="123" t="s">
         <v>159</v>
       </c>
-      <c r="M6" s="152">
-        <f>EXP(lambda_L*B6)</f>
+      <c r="M6" s="138">
+        <f t="shared" si="0"/>
         <v>1.0575976837366112</v>
       </c>
-      <c r="N6" s="152">
-        <f>EXP(lambda_E*B6)</f>
+      <c r="N6" s="138">
+        <f t="shared" si="1"/>
         <v>1.0898063283051287</v>
       </c>
       <c r="O6" s="123">
-        <f>E6^alpha * (M6*D6)^beta</f>
+        <f t="shared" si="2"/>
         <v>1.118810046641995</v>
       </c>
       <c r="P6" s="123">
-        <f>((1-gamma_E)^1 * O6^phi + gamma_E^1 * ($N6*F6)^phi)^invPhi</f>
+        <f t="shared" si="3"/>
         <v>1.1186468206858819</v>
       </c>
       <c r="Q6" s="123">
-        <f>((1-gamma_E)^1 * P6^phi + gamma_E^1 * ($N6*G6)^phi)^invPhi</f>
+        <f t="shared" si="4"/>
         <v>1.1184827499997807</v>
       </c>
       <c r="R6" s="123">
-        <f>((1-gamma_E)^1 * Q6^phi + gamma_E^1 * ($N6*H6)^phi)^invPhi</f>
+        <f t="shared" si="5"/>
         <v>1.1183069963859926</v>
       </c>
     </row>
@@ -30034,28 +30038,28 @@
       <c r="L7" s="123" t="s">
         <v>160</v>
       </c>
-      <c r="M7" s="152">
-        <f>EXP(lambda_L*B7)</f>
+      <c r="M7" s="138">
+        <f t="shared" si="0"/>
         <v>1.0725081812542165</v>
       </c>
-      <c r="N7" s="152">
-        <f>EXP(lambda_E*B7)</f>
+      <c r="N7" s="138">
+        <f t="shared" si="1"/>
         <v>1.1134908607465361</v>
       </c>
       <c r="O7" s="123">
-        <f>E7^alpha * (M7*D7)^beta</f>
+        <f t="shared" si="2"/>
         <v>1.1617640869622503</v>
       </c>
       <c r="P7" s="123">
-        <f>((1-gamma_E)^1 * O7^phi + gamma_E^1 * ($N7*F7)^phi)^invPhi</f>
+        <f t="shared" si="3"/>
         <v>1.1615797656379097</v>
       </c>
       <c r="Q7" s="123">
-        <f>((1-gamma_E)^1 * P7^phi + gamma_E^1 * ($N7*G7)^phi)^invPhi</f>
+        <f t="shared" si="4"/>
         <v>1.1613950569165381</v>
       </c>
       <c r="R7" s="123">
-        <f>((1-gamma_E)^1 * Q7^phi + gamma_E^1 * ($N7*H7)^phi)^invPhi</f>
+        <f t="shared" si="5"/>
         <v>1.1612104564787413</v>
       </c>
     </row>
@@ -30102,28 +30106,28 @@
       <c r="L8" s="123" t="s">
         <v>161</v>
       </c>
-      <c r="M8" s="152">
-        <f>EXP(lambda_L*B8)</f>
+      <c r="M8" s="138">
+        <f t="shared" si="0"/>
         <v>1.0876288938088261</v>
       </c>
-      <c r="N8" s="152">
-        <f>EXP(lambda_E*B8)</f>
+      <c r="N8" s="138">
+        <f t="shared" si="1"/>
         <v>1.1376901241657316</v>
       </c>
       <c r="O8" s="123">
-        <f>E8^alpha * (M8*D8)^beta</f>
+        <f t="shared" si="2"/>
         <v>1.1959986897647981</v>
       </c>
       <c r="P8" s="123">
-        <f>((1-gamma_E)^1 * O8^phi + gamma_E^1 * ($N8*F8)^phi)^invPhi</f>
+        <f t="shared" si="3"/>
         <v>1.1958062473635533</v>
       </c>
       <c r="Q8" s="123">
-        <f>((1-gamma_E)^1 * P8^phi + gamma_E^1 * ($N8*G8)^phi)^invPhi</f>
+        <f t="shared" si="4"/>
         <v>1.195613438838903</v>
       </c>
       <c r="R8" s="123">
-        <f>((1-gamma_E)^1 * Q8^phi + gamma_E^1 * ($N8*H8)^phi)^invPhi</f>
+        <f t="shared" si="5"/>
         <v>1.1954167121773991</v>
       </c>
     </row>
@@ -30167,28 +30171,28 @@
         <f>1-K3</f>
         <v>0.27400000000000002</v>
       </c>
-      <c r="M9" s="152">
-        <f>EXP(lambda_L*B9)</f>
+      <c r="M9" s="138">
+        <f t="shared" si="0"/>
         <v>1.1029627851085078</v>
       </c>
-      <c r="N9" s="152">
-        <f>EXP(lambda_E*B9)</f>
+      <c r="N9" s="138">
+        <f t="shared" si="1"/>
         <v>1.1624153051031354</v>
       </c>
       <c r="O9" s="123">
-        <f>E9^alpha * (M9*D9)^beta</f>
+        <f t="shared" si="2"/>
         <v>1.2438456543998093</v>
       </c>
       <c r="P9" s="123">
-        <f>((1-gamma_E)^1 * O9^phi + gamma_E^1 * ($N9*F9)^phi)^invPhi</f>
+        <f t="shared" si="3"/>
         <v>1.2436555272562895</v>
       </c>
       <c r="Q9" s="123">
-        <f>((1-gamma_E)^1 * P9^phi + gamma_E^1 * ($N9*G9)^phi)^invPhi</f>
+        <f t="shared" si="4"/>
         <v>1.2434648204059637</v>
       </c>
       <c r="R9" s="123">
-        <f>((1-gamma_E)^1 * Q9^phi + gamma_E^1 * ($N9*H9)^phi)^invPhi</f>
+        <f t="shared" si="5"/>
         <v>1.2432683685025845</v>
       </c>
     </row>
@@ -30225,28 +30229,28 @@
         <f>USData!H10</f>
         <v>1.0731648261553837</v>
       </c>
-      <c r="M10" s="152">
-        <f>EXP(lambda_L*B10)</f>
+      <c r="M10" s="138">
+        <f t="shared" si="0"/>
         <v>1.1185128606450452</v>
       </c>
-      <c r="N10" s="152">
-        <f>EXP(lambda_E*B10)</f>
+      <c r="N10" s="138">
+        <f t="shared" si="1"/>
         <v>1.187677833213906</v>
       </c>
       <c r="O10" s="123">
-        <f>E10^alpha * (M10*D10)^beta</f>
+        <f t="shared" si="2"/>
         <v>1.2959506948180715</v>
       </c>
       <c r="P10" s="123">
-        <f>((1-gamma_E)^1 * O10^phi + gamma_E^1 * ($N10*F10)^phi)^invPhi</f>
+        <f t="shared" si="3"/>
         <v>1.2957939540283201</v>
       </c>
       <c r="Q10" s="123">
-        <f>((1-gamma_E)^1 * P10^phi + gamma_E^1 * ($N10*G10)^phi)^invPhi</f>
+        <f t="shared" si="4"/>
         <v>1.2956355493647942</v>
       </c>
       <c r="R10" s="123">
-        <f>((1-gamma_E)^1 * Q10^phi + gamma_E^1 * ($N10*H10)^phi)^invPhi</f>
+        <f t="shared" si="5"/>
         <v>1.2955271333901193</v>
       </c>
     </row>
@@ -30283,28 +30287,28 @@
         <f>USData!H11</f>
         <v>1.132762084079274</v>
       </c>
-      <c r="M11" s="152">
-        <f>EXP(lambda_L*B11)</f>
+      <c r="M11" s="138">
+        <f t="shared" si="0"/>
         <v>1.1342821682830251</v>
       </c>
-      <c r="N11" s="152">
-        <f>EXP(lambda_E*B11)</f>
+      <c r="N11" s="138">
+        <f t="shared" si="1"/>
         <v>1.2134893865514997</v>
       </c>
       <c r="O11" s="123">
-        <f>E11^alpha * (M11*D11)^beta</f>
+        <f t="shared" si="2"/>
         <v>1.3480210435078956</v>
       </c>
       <c r="P11" s="123">
-        <f>((1-gamma_E)^1 * O11^phi + gamma_E^1 * ($N11*F11)^phi)^invPhi</f>
+        <f t="shared" si="3"/>
         <v>1.3479025060598049</v>
       </c>
       <c r="Q11" s="123">
-        <f>((1-gamma_E)^1 * P11^phi + gamma_E^1 * ($N11*G11)^phi)^invPhi</f>
+        <f t="shared" si="4"/>
         <v>1.3477770577594308</v>
       </c>
       <c r="R11" s="123">
-        <f>((1-gamma_E)^1 * Q11^phi + gamma_E^1 * ($N11*H11)^phi)^invPhi</f>
+        <f t="shared" si="5"/>
         <v>1.3480618663282531</v>
       </c>
     </row>
@@ -30341,28 +30345,28 @@
         <f>USData!H12</f>
         <v>1.1515878312567835</v>
       </c>
-      <c r="M12" s="152">
-        <f>EXP(lambda_L*B12)</f>
+      <c r="M12" s="138">
+        <f t="shared" si="0"/>
         <v>1.1502737988572274</v>
       </c>
-      <c r="N12" s="152">
-        <f>EXP(lambda_E*B12)</f>
+      <c r="N12" s="138">
+        <f t="shared" si="1"/>
         <v>1.2398618969660617</v>
       </c>
       <c r="O12" s="123">
-        <f>E12^alpha * (M12*D12)^beta</f>
+        <f t="shared" si="2"/>
         <v>1.3748755368458783</v>
       </c>
       <c r="P12" s="123">
-        <f>((1-gamma_E)^1 * O12^phi + gamma_E^1 * ($N12*F12)^phi)^invPhi</f>
+        <f t="shared" si="3"/>
         <v>1.3747933249920963</v>
       </c>
       <c r="Q12" s="123">
-        <f>((1-gamma_E)^1 * P12^phi + gamma_E^1 * ($N12*G12)^phi)^invPhi</f>
+        <f t="shared" si="4"/>
         <v>1.3746976473463661</v>
       </c>
       <c r="R12" s="123">
-        <f>((1-gamma_E)^1 * Q12^phi + gamma_E^1 * ($N12*H12)^phi)^invPhi</f>
+        <f t="shared" si="5"/>
         <v>1.3755624562599085</v>
       </c>
     </row>
@@ -30399,28 +30403,28 @@
         <f>USData!H13</f>
         <v>1.1388630838040485</v>
       </c>
-      <c r="M13" s="152">
-        <f>EXP(lambda_L*B13)</f>
+      <c r="M13" s="138">
+        <f t="shared" si="0"/>
         <v>1.1664908867784396</v>
       </c>
-      <c r="N13" s="152">
-        <f>EXP(lambda_E*B13)</f>
+      <c r="N13" s="138">
+        <f t="shared" si="1"/>
         <v>1.2668075556201339</v>
       </c>
       <c r="O13" s="123">
-        <f>E13^alpha * (M13*D13)^beta</f>
+        <f t="shared" si="2"/>
         <v>1.3831632243924659</v>
       </c>
       <c r="P13" s="123">
-        <f>((1-gamma_E)^1 * O13^phi + gamma_E^1 * ($N13*F13)^phi)^invPhi</f>
+        <f t="shared" si="3"/>
         <v>1.3832137716976249</v>
       </c>
       <c r="Q13" s="123">
-        <f>((1-gamma_E)^1 * P13^phi + gamma_E^1 * ($N13*G13)^phi)^invPhi</f>
+        <f t="shared" si="4"/>
         <v>1.3832341216856923</v>
       </c>
       <c r="R13" s="123">
-        <f>((1-gamma_E)^1 * Q13^phi + gamma_E^1 * ($N13*H13)^phi)^invPhi</f>
+        <f t="shared" si="5"/>
         <v>1.3843083616339238</v>
       </c>
     </row>
@@ -30457,28 +30461,28 @@
         <f>USData!H14</f>
         <v>1.1874189587884159</v>
       </c>
-      <c r="M14" s="152">
-        <f>EXP(lambda_L*B14)</f>
+      <c r="M14" s="138">
+        <f t="shared" si="0"/>
         <v>1.1829366106478107</v>
       </c>
-      <c r="N14" s="152">
-        <f>EXP(lambda_E*B14)</f>
+      <c r="N14" s="138">
+        <f t="shared" si="1"/>
         <v>1.2943388186242377</v>
       </c>
       <c r="O14" s="123">
-        <f>E14^alpha * (M14*D14)^beta</f>
+        <f t="shared" si="2"/>
         <v>1.407864557586376</v>
       </c>
       <c r="P14" s="123">
-        <f>((1-gamma_E)^1 * O14^phi + gamma_E^1 * ($N14*F14)^phi)^invPhi</f>
+        <f t="shared" si="3"/>
         <v>1.4082301382342552</v>
       </c>
       <c r="Q14" s="123">
-        <f>((1-gamma_E)^1 * P14^phi + gamma_E^1 * ($N14*G14)^phi)^invPhi</f>
+        <f t="shared" si="4"/>
         <v>1.4085315460038599</v>
       </c>
       <c r="R14" s="123">
-        <f>((1-gamma_E)^1 * Q14^phi + gamma_E^1 * ($N14*H14)^phi)^invPhi</f>
+        <f t="shared" si="5"/>
         <v>1.4160317854407301</v>
       </c>
     </row>
@@ -30515,28 +30519,28 @@
         <f>USData!H15</f>
         <v>1.1995642582030086</v>
       </c>
-      <c r="M15" s="152">
-        <f>EXP(lambda_L*B15)</f>
+      <c r="M15" s="138">
+        <f t="shared" si="0"/>
         <v>1.1996141938798683</v>
       </c>
-      <c r="N15" s="152">
-        <f>EXP(lambda_E*B15)</f>
+      <c r="N15" s="138">
+        <f t="shared" si="1"/>
         <v>1.3224684127949329</v>
       </c>
       <c r="O15" s="123">
-        <f>E15^alpha * (M15*D15)^beta</f>
+        <f t="shared" si="2"/>
         <v>1.4580450868502455</v>
       </c>
       <c r="P15" s="123">
-        <f>((1-gamma_E)^1 * O15^phi + gamma_E^1 * ($N15*F15)^phi)^invPhi</f>
+        <f t="shared" si="3"/>
         <v>1.4585823658919383</v>
       </c>
       <c r="Q15" s="123">
-        <f>((1-gamma_E)^1 * P15^phi + gamma_E^1 * ($N15*G15)^phi)^invPhi</f>
+        <f t="shared" si="4"/>
         <v>1.45903325052458</v>
       </c>
       <c r="R15" s="123">
-        <f>((1-gamma_E)^1 * Q15^phi + gamma_E^1 * ($N15*H15)^phi)^invPhi</f>
+        <f t="shared" si="5"/>
         <v>1.465813727971905</v>
       </c>
     </row>
@@ -30573,28 +30577,28 @@
         <f>USData!H16</f>
         <v>1.2387054028291842</v>
       </c>
-      <c r="M16" s="152">
-        <f>EXP(lambda_L*B16)</f>
+      <c r="M16" s="138">
+        <f t="shared" si="0"/>
         <v>1.2165269053343162</v>
       </c>
-      <c r="N16" s="152">
-        <f>EXP(lambda_E*B16)</f>
+      <c r="N16" s="138">
+        <f t="shared" si="1"/>
         <v>1.3512093415380155</v>
       </c>
       <c r="O16" s="123">
-        <f>E16^alpha * (M16*D16)^beta</f>
+        <f t="shared" si="2"/>
         <v>1.5204090274417355</v>
       </c>
       <c r="P16" s="123">
-        <f>((1-gamma_E)^1 * O16^phi + gamma_E^1 * ($N16*F16)^phi)^invPhi</f>
+        <f t="shared" si="3"/>
         <v>1.5209334832863295</v>
       </c>
       <c r="Q16" s="123">
-        <f>((1-gamma_E)^1 * P16^phi + gamma_E^1 * ($N16*G16)^phi)^invPhi</f>
+        <f t="shared" si="4"/>
         <v>1.5213719754703734</v>
       </c>
       <c r="R16" s="123">
-        <f>((1-gamma_E)^1 * Q16^phi + gamma_E^1 * ($N16*H16)^phi)^invPhi</f>
+        <f t="shared" si="5"/>
         <v>1.5323700014114352</v>
       </c>
     </row>
@@ -30631,28 +30635,28 @@
         <f>USData!H17</f>
         <v>1.2919642899061348</v>
       </c>
-      <c r="M17" s="152">
-        <f>EXP(lambda_L*B17)</f>
+      <c r="M17" s="138">
+        <f t="shared" si="0"/>
         <v>1.2336780599567432</v>
       </c>
-      <c r="N17" s="152">
-        <f>EXP(lambda_E*B17)</f>
+      <c r="N17" s="138">
+        <f t="shared" si="1"/>
         <v>1.3805748908595732</v>
       </c>
       <c r="O17" s="123">
-        <f>E17^alpha * (M17*D17)^beta</f>
+        <f t="shared" si="2"/>
         <v>1.5791838766471218</v>
       </c>
       <c r="P17" s="123">
-        <f>((1-gamma_E)^1 * O17^phi + gamma_E^1 * ($N17*F17)^phi)^invPhi</f>
+        <f t="shared" si="3"/>
         <v>1.5799261041795343</v>
       </c>
       <c r="Q17" s="123">
-        <f>((1-gamma_E)^1 * P17^phi + gamma_E^1 * ($N17*G17)^phi)^invPhi</f>
+        <f t="shared" si="4"/>
         <v>1.5805307983871659</v>
       </c>
       <c r="R17" s="123">
-        <f>((1-gamma_E)^1 * Q17^phi + gamma_E^1 * ($N17*H17)^phi)^invPhi</f>
+        <f t="shared" si="5"/>
         <v>1.6072462701191914</v>
       </c>
     </row>
@@ -30689,28 +30693,28 @@
         <f>USData!H18</f>
         <v>1.3335423024180206</v>
       </c>
-      <c r="M18" s="152">
-        <f>EXP(lambda_L*B18)</f>
+      <c r="M18" s="138">
+        <f t="shared" si="0"/>
         <v>1.2510710194283623</v>
       </c>
-      <c r="N18" s="152">
-        <f>EXP(lambda_E*B18)</f>
+      <c r="N18" s="138">
+        <f t="shared" si="1"/>
         <v>1.4105786355076784</v>
       </c>
       <c r="O18" s="123">
-        <f>E18^alpha * (M18*D18)^beta</f>
+        <f t="shared" si="2"/>
         <v>1.628399752153936</v>
       </c>
       <c r="P18" s="123">
-        <f>((1-gamma_E)^1 * O18^phi + gamma_E^1 * ($N18*F18)^phi)^invPhi</f>
+        <f t="shared" si="3"/>
         <v>1.6307284911297213</v>
       </c>
       <c r="Q18" s="123">
-        <f>((1-gamma_E)^1 * P18^phi + gamma_E^1 * ($N18*G18)^phi)^invPhi</f>
+        <f t="shared" si="4"/>
         <v>1.6326459067009078</v>
       </c>
       <c r="R18" s="123">
-        <f>((1-gamma_E)^1 * Q18^phi + gamma_E^1 * ($N18*H18)^phi)^invPhi</f>
+        <f t="shared" si="5"/>
         <v>1.6811550747054322</v>
       </c>
     </row>
@@ -30747,28 +30751,28 @@
         <f>USData!H19</f>
         <v>1.3522881805788678</v>
       </c>
-      <c r="M19" s="152">
-        <f>EXP(lambda_L*B19)</f>
+      <c r="M19" s="138">
+        <f t="shared" si="0"/>
         <v>1.2687091928249108</v>
       </c>
-      <c r="N19" s="152">
-        <f>EXP(lambda_E*B19)</f>
+      <c r="N19" s="138">
+        <f t="shared" si="1"/>
         <v>1.4412344452475572</v>
       </c>
       <c r="O19" s="123">
-        <f>E19^alpha * (M19*D19)^beta</f>
+        <f t="shared" si="2"/>
         <v>1.7017232981524548</v>
       </c>
       <c r="P19" s="123">
-        <f>((1-gamma_E)^1 * O19^phi + gamma_E^1 * ($N19*F19)^phi)^invPhi</f>
+        <f t="shared" si="3"/>
         <v>1.7029795236792338</v>
       </c>
       <c r="Q19" s="123">
-        <f>((1-gamma_E)^1 * P19^phi + gamma_E^1 * ($N19*G19)^phi)^invPhi</f>
+        <f t="shared" si="4"/>
         <v>1.704042984943352</v>
       </c>
       <c r="R19" s="123">
-        <f>((1-gamma_E)^1 * Q19^phi + gamma_E^1 * ($N19*H19)^phi)^invPhi</f>
+        <f t="shared" si="5"/>
         <v>1.7460845792467194</v>
       </c>
     </row>
@@ -30805,28 +30809,28 @@
         <f>USData!H20</f>
         <v>1.3668763473090262</v>
       </c>
-      <c r="M20" s="152">
-        <f>EXP(lambda_L*B20)</f>
+      <c r="M20" s="138">
+        <f t="shared" si="0"/>
         <v>1.2865960372848406</v>
       </c>
-      <c r="N20" s="152">
-        <f>EXP(lambda_E*B20)</f>
+      <c r="N20" s="138">
+        <f t="shared" si="1"/>
         <v>1.4725564912731353</v>
       </c>
       <c r="O20" s="123">
-        <f>E20^alpha * (M20*D20)^beta</f>
+        <f t="shared" si="2"/>
         <v>1.7717267491093867</v>
       </c>
       <c r="P20" s="123">
-        <f>((1-gamma_E)^1 * O20^phi + gamma_E^1 * ($N20*F20)^phi)^invPhi</f>
+        <f t="shared" si="3"/>
         <v>1.7724064362271621</v>
       </c>
       <c r="Q20" s="123">
-        <f>((1-gamma_E)^1 * P20^phi + gamma_E^1 * ($N20*G20)^phi)^invPhi</f>
+        <f t="shared" si="4"/>
         <v>1.7729783328829083</v>
       </c>
       <c r="R20" s="123">
-        <f>((1-gamma_E)^1 * Q20^phi + gamma_E^1 * ($N20*H20)^phi)^invPhi</f>
+        <f t="shared" si="5"/>
         <v>1.8086661664064663</v>
       </c>
     </row>
@@ -30863,28 +30867,28 @@
         <f>USData!H21</f>
         <v>1.4091187520234514</v>
       </c>
-      <c r="M21" s="152">
-        <f>EXP(lambda_L*B21)</f>
+      <c r="M21" s="138">
+        <f t="shared" si="0"/>
         <v>1.304735058686928</v>
       </c>
-      <c r="N21" s="152">
-        <f>EXP(lambda_E*B21)</f>
+      <c r="N21" s="138">
+        <f t="shared" si="1"/>
         <v>1.5045592527579252</v>
       </c>
       <c r="O21" s="123">
-        <f>E21^alpha * (M21*D21)^beta</f>
+        <f t="shared" si="2"/>
         <v>1.8441911279784078</v>
       </c>
       <c r="P21" s="123">
-        <f>((1-gamma_E)^1 * O21^phi + gamma_E^1 * ($N21*F21)^phi)^invPhi</f>
+        <f t="shared" si="3"/>
         <v>1.8447987851443208</v>
       </c>
       <c r="Q21" s="123">
-        <f>((1-gamma_E)^1 * P21^phi + gamma_E^1 * ($N21*G21)^phi)^invPhi</f>
+        <f t="shared" si="4"/>
         <v>1.8452989159947781</v>
       </c>
       <c r="R21" s="123">
-        <f>((1-gamma_E)^1 * Q21^phi + gamma_E^1 * ($N21*H21)^phi)^invPhi</f>
+        <f t="shared" si="5"/>
         <v>1.8964476649164279</v>
       </c>
     </row>
@@ -30903,7 +30907,7 @@
       </c>
       <c r="D22" s="123">
         <f>USData!D22</f>
-        <v>1.3958740924307638</v>
+        <v>1.395874092430764</v>
       </c>
       <c r="E22" s="123">
         <f>USData!E22</f>
@@ -30921,28 +30925,28 @@
         <f>USData!H22</f>
         <v>1.3964447355801066</v>
       </c>
-      <c r="M22" s="152">
-        <f>EXP(lambda_L*B22)</f>
+      <c r="M22" s="138">
+        <f t="shared" si="0"/>
         <v>1.3231298123374369</v>
       </c>
-      <c r="N22" s="152">
-        <f>EXP(lambda_E*B22)</f>
+      <c r="N22" s="138">
+        <f t="shared" si="1"/>
         <v>1.5372575235482813</v>
       </c>
       <c r="O22" s="123">
-        <f>E22^alpha * (M22*D22)^beta</f>
+        <f t="shared" si="2"/>
         <v>1.9119530966962257</v>
       </c>
       <c r="P22" s="123">
-        <f>((1-gamma_E)^1 * O22^phi + gamma_E^1 * ($N22*F22)^phi)^invPhi</f>
+        <f t="shared" si="3"/>
         <v>1.9128560525642373</v>
       </c>
       <c r="Q22" s="123">
-        <f>((1-gamma_E)^1 * P22^phi + gamma_E^1 * ($N22*G22)^phi)^invPhi</f>
+        <f t="shared" si="4"/>
         <v>1.9136189768293614</v>
       </c>
       <c r="R22" s="123">
-        <f>((1-gamma_E)^1 * Q22^phi + gamma_E^1 * ($N22*H22)^phi)^invPhi</f>
+        <f t="shared" si="5"/>
         <v>1.9405119932307708</v>
       </c>
     </row>
@@ -30979,24 +30983,24 @@
         <f>USData!H23</f>
         <v>NA</v>
       </c>
-      <c r="M23" s="152">
-        <f>EXP(lambda_L*B23)</f>
+      <c r="M23" s="138">
+        <f t="shared" si="0"/>
         <v>1.3417839036669714</v>
       </c>
-      <c r="N23" s="152">
-        <f>EXP(lambda_E*B23)</f>
+      <c r="N23" s="138">
+        <f t="shared" si="1"/>
         <v>1.5706664190021191</v>
       </c>
       <c r="O23" s="123">
-        <f>E23^alpha * (M23*D23)^beta</f>
+        <f t="shared" si="2"/>
         <v>1.940796506358619</v>
       </c>
       <c r="P23" s="123">
-        <f>((1-gamma_E)^1 * O23^phi + gamma_E^1 * ($N23*F23)^phi)^invPhi</f>
+        <f t="shared" ref="P23:P33" si="6">((1-gamma_E)^1 * O23^phi + gamma_E^1 * ($N23*F23)^phi)^invPhi</f>
         <v>1.9410869139354936</v>
       </c>
       <c r="Q23" s="123">
-        <f>((1-gamma_E)^1 * P23^phi + gamma_E^1 * ($N23*G23)^phi)^invPhi</f>
+        <f t="shared" ref="Q23:Q33" si="7">((1-gamma_E)^1 * P23^phi + gamma_E^1 * ($N23*G23)^phi)^invPhi</f>
         <v>1.941311580975815</v>
       </c>
       <c r="R23" s="123"/>
@@ -31034,24 +31038,24 @@
         <f>USData!H24</f>
         <v>NA</v>
       </c>
-      <c r="M24" s="152">
-        <f>EXP(lambda_L*B24)</f>
+      <c r="M24" s="138">
+        <f t="shared" si="0"/>
         <v>1.3607009889371502</v>
       </c>
-      <c r="N24" s="152">
-        <f>EXP(lambda_E*B24)</f>
+      <c r="N24" s="138">
+        <f t="shared" si="1"/>
         <v>1.6048013829762589</v>
       </c>
       <c r="O24" s="123">
-        <f>E24^alpha * (M24*D24)^beta</f>
+        <f t="shared" si="2"/>
         <v>1.9633465485969452</v>
       </c>
       <c r="P24" s="123">
-        <f>((1-gamma_E)^1 * O24^phi + gamma_E^1 * ($N24*F24)^phi)^invPhi</f>
+        <f t="shared" si="6"/>
         <v>1.9649820658088395</v>
       </c>
       <c r="Q24" s="123">
-        <f>((1-gamma_E)^1 * P24^phi + gamma_E^1 * ($N24*G24)^phi)^invPhi</f>
+        <f t="shared" si="7"/>
         <v>1.966331666465913</v>
       </c>
       <c r="R24" s="123"/>
@@ -31089,24 +31093,24 @@
         <f>USData!H25</f>
         <v>NA</v>
       </c>
-      <c r="M25" s="152">
-        <f>EXP(lambda_L*B25)</f>
+      <c r="M25" s="138">
+        <f t="shared" si="0"/>
         <v>1.3798847759572466</v>
       </c>
-      <c r="N25" s="152">
-        <f>EXP(lambda_E*B25)</f>
+      <c r="N25" s="138">
+        <f t="shared" si="1"/>
         <v>1.6396781949656225</v>
       </c>
       <c r="O25" s="123">
-        <f>E25^alpha * (M25*D25)^beta</f>
+        <f t="shared" si="2"/>
         <v>1.9972917768058769</v>
       </c>
       <c r="P25" s="123">
-        <f>((1-gamma_E)^1 * O25^phi + gamma_E^1 * ($N25*F25)^phi)^invPhi</f>
+        <f t="shared" si="6"/>
         <v>1.9995546343483528</v>
       </c>
       <c r="Q25" s="123">
-        <f>((1-gamma_E)^1 * P25^phi + gamma_E^1 * ($N25*G25)^phi)^invPhi</f>
+        <f t="shared" si="7"/>
         <v>2.0014276737644066</v>
       </c>
       <c r="R25" s="123"/>
@@ -31144,24 +31148,24 @@
         <f>USData!H26</f>
         <v>NA</v>
       </c>
-      <c r="M26" s="152">
-        <f>EXP(lambda_L*B26)</f>
+      <c r="M26" s="138">
+        <f t="shared" si="0"/>
         <v>1.3993390248109305</v>
       </c>
-      <c r="N26" s="152">
-        <f>EXP(lambda_E*B26)</f>
+      <c r="N26" s="138">
+        <f t="shared" si="1"/>
         <v>1.6753129773975874</v>
       </c>
       <c r="O26" s="123">
-        <f>E26^alpha * (M26*D26)^beta</f>
+        <f t="shared" si="2"/>
         <v>2.0580640683865337</v>
       </c>
       <c r="P26" s="123">
-        <f>((1-gamma_E)^1 * O26^phi + gamma_E^1 * ($N26*F26)^phi)^invPhi</f>
+        <f t="shared" si="6"/>
         <v>2.061386958998451</v>
       </c>
       <c r="Q26" s="123">
-        <f>((1-gamma_E)^1 * P26^phi + gamma_E^1 * ($N26*G26)^phi)^invPhi</f>
+        <f t="shared" si="7"/>
         <v>2.0641215142971117</v>
       </c>
       <c r="R26" s="123"/>
@@ -31199,24 +31203,24 @@
         <f>USData!H27</f>
         <v>NA</v>
       </c>
-      <c r="M27" s="152">
-        <f>EXP(lambda_L*B27)</f>
+      <c r="M27" s="138">
+        <f t="shared" si="0"/>
         <v>1.4190675485932573</v>
       </c>
-      <c r="N27" s="152">
-        <f>EXP(lambda_E*B27)</f>
+      <c r="N27" s="138">
+        <f t="shared" si="1"/>
         <v>1.7117222030848642</v>
       </c>
       <c r="O27" s="123">
-        <f>E27^alpha * (M27*D27)^beta</f>
+        <f t="shared" si="2"/>
         <v>2.1283216373394844</v>
       </c>
       <c r="P27" s="123">
-        <f>((1-gamma_E)^1 * O27^phi + gamma_E^1 * ($N27*F27)^phi)^invPhi</f>
+        <f t="shared" si="6"/>
         <v>2.13043897797295</v>
       </c>
       <c r="Q27" s="123">
-        <f>((1-gamma_E)^1 * P27^phi + gamma_E^1 * ($N27*G27)^phi)^invPhi</f>
+        <f t="shared" si="7"/>
         <v>2.1321915962558844</v>
       </c>
       <c r="R27" s="123"/>
@@ -31254,24 +31258,24 @@
         <f>USData!H28</f>
         <v>NA</v>
       </c>
-      <c r="M28" s="152">
-        <f>EXP(lambda_L*B28)</f>
+      <c r="M28" s="138">
+        <f t="shared" si="0"/>
         <v>1.4390742141580464</v>
       </c>
-      <c r="N28" s="152">
-        <f>EXP(lambda_E*B28)</f>
+      <c r="N28" s="138">
+        <f t="shared" si="1"/>
         <v>1.7489227028403491</v>
       </c>
       <c r="O28" s="123">
-        <f>E28^alpha * (M28*D28)^beta</f>
+        <f t="shared" si="2"/>
         <v>2.204099675454867</v>
       </c>
       <c r="P28" s="123">
-        <f>((1-gamma_E)^1 * O28^phi + gamma_E^1 * ($N28*F28)^phi)^invPhi</f>
+        <f t="shared" si="6"/>
         <v>2.2049028499886405</v>
       </c>
       <c r="Q28" s="123">
-        <f>((1-gamma_E)^1 * P28^phi + gamma_E^1 * ($N28*G28)^phi)^invPhi</f>
+        <f t="shared" si="7"/>
         <v>2.2055366663613434</v>
       </c>
       <c r="R28" s="123"/>
@@ -31291,7 +31295,7 @@
       </c>
       <c r="D29" s="123">
         <f>USData!D29</f>
-        <v>1.4253238989609147</v>
+        <v>1.4252423807660537</v>
       </c>
       <c r="E29" s="123">
         <f>USData!E29</f>
@@ -31309,25 +31313,25 @@
         <f>USData!H29</f>
         <v>NA</v>
       </c>
-      <c r="M29" s="152">
-        <f>EXP(lambda_L*B29)</f>
+      <c r="M29" s="138">
+        <f t="shared" si="0"/>
         <v>1.4593629428757966</v>
       </c>
-      <c r="N29" s="152">
-        <f>EXP(lambda_E*B29)</f>
+      <c r="N29" s="138">
+        <f t="shared" si="1"/>
         <v>1.7869316732574658</v>
       </c>
       <c r="O29" s="123">
-        <f>E29^alpha * (M29*D29)^beta</f>
-        <v>2.2600276513888584</v>
+        <f t="shared" si="2"/>
+        <v>2.2599338099272752</v>
       </c>
       <c r="P29" s="123">
-        <f>((1-gamma_E)^1 * O29^phi + gamma_E^1 * ($N29*F29)^phi)^invPhi</f>
-        <v>2.2616989357881314</v>
+        <f t="shared" si="6"/>
+        <v>2.2616084690041798</v>
       </c>
       <c r="Q29" s="123">
-        <f>((1-gamma_E)^1 * P29^phi + gamma_E^1 * ($N29*G29)^phi)^invPhi</f>
-        <v>2.263045948176289</v>
+        <f t="shared" si="7"/>
+        <v>2.2629582310254754</v>
       </c>
       <c r="R29" s="123"/>
     </row>
@@ -31346,7 +31350,7 @@
       </c>
       <c r="D30" s="123">
         <f>USData!D30</f>
-        <v>1.4099386983174644</v>
+        <v>1.4100365201512979</v>
       </c>
       <c r="E30" s="123">
         <f>USData!E30</f>
@@ -31364,25 +31368,25 @@
         <f>USData!H30</f>
         <v>NA</v>
       </c>
-      <c r="M30" s="152">
-        <f>EXP(lambda_L*B30)</f>
+      <c r="M30" s="138">
+        <f t="shared" si="0"/>
         <v>1.4799377114022885</v>
       </c>
-      <c r="N30" s="152">
-        <f>EXP(lambda_E*B30)</f>
+      <c r="N30" s="138">
+        <f t="shared" si="1"/>
         <v>1.8257666846595977</v>
       </c>
       <c r="O30" s="123">
-        <f>E30^alpha * (M30*D30)^beta</f>
-        <v>2.280916357906436</v>
+        <f t="shared" si="2"/>
+        <v>2.281031246634678</v>
       </c>
       <c r="P30" s="123">
-        <f>((1-gamma_E)^1 * O30^phi + gamma_E^1 * ($N30*F30)^phi)^invPhi</f>
-        <v>2.2818543088894514</v>
+        <f t="shared" si="6"/>
+        <v>2.2819665352527334</v>
       </c>
       <c r="Q30" s="123">
-        <f>((1-gamma_E)^1 * P30^phi + gamma_E^1 * ($N30*G30)^phi)^invPhi</f>
-        <v>2.2825619266122987</v>
+        <f t="shared" si="7"/>
+        <v>2.2826719959151704</v>
       </c>
       <c r="R30" s="123"/>
     </row>
@@ -31401,7 +31405,7 @@
       </c>
       <c r="D31" s="123">
         <f>USData!D31</f>
-        <v>1.3323170731707317</v>
+        <v>1.3320833876787965</v>
       </c>
       <c r="E31" s="123">
         <f>USData!E31</f>
@@ -31419,25 +31423,25 @@
         <f>USData!H31</f>
         <v>NA</v>
       </c>
-      <c r="M31" s="152">
-        <f>EXP(lambda_L*B31)</f>
+      <c r="M31" s="138">
+        <f t="shared" si="0"/>
         <v>1.50080255245802</v>
       </c>
-      <c r="N31" s="152">
-        <f>EXP(lambda_E*B31)</f>
+      <c r="N31" s="138">
+        <f t="shared" si="1"/>
         <v>1.8654456892222817</v>
       </c>
       <c r="O31" s="123">
-        <f>E31^alpha * (M31*D31)^beta</f>
-        <v>2.2148252234317427</v>
+        <f t="shared" si="2"/>
+        <v>2.2145431834516218</v>
       </c>
       <c r="P31" s="123">
-        <f>((1-gamma_E)^1 * O31^phi + gamma_E^1 * ($N31*F31)^phi)^invPhi</f>
-        <v>2.2160813457043989</v>
+        <f t="shared" si="6"/>
+        <v>2.2158075810351896</v>
       </c>
       <c r="Q31" s="123">
-        <f>((1-gamma_E)^1 * P31^phi + gamma_E^1 * ($N31*G31)^phi)^invPhi</f>
-        <v>2.2169806645566514</v>
+        <f t="shared" si="7"/>
+        <v>2.2167132080181866</v>
       </c>
       <c r="R31" s="123"/>
     </row>
@@ -31456,7 +31460,7 @@
       </c>
       <c r="D32" s="123">
         <f>USData!D32</f>
-        <v>1.3317627494456763</v>
+        <v>1.3321431676883613</v>
       </c>
       <c r="E32" s="123">
         <f>USData!E32</f>
@@ -31474,25 +31478,25 @@
         <f>USData!H32</f>
         <v>NA</v>
       </c>
-      <c r="M32" s="152">
-        <f>EXP(lambda_L*B32)</f>
+      <c r="M32" s="138">
+        <f t="shared" si="0"/>
         <v>1.5219615556186337</v>
       </c>
-      <c r="N32" s="152">
-        <f>EXP(lambda_E*B32)</f>
+      <c r="N32" s="138">
+        <f t="shared" si="1"/>
         <v>1.9059870292719225</v>
       </c>
       <c r="O32" s="123">
-        <f>E32^alpha * (M32*D32)^beta</f>
-        <v>2.2411706361689756</v>
+        <f t="shared" si="2"/>
+        <v>2.2416353964678675</v>
       </c>
       <c r="P32" s="123">
-        <f>((1-gamma_E)^1 * O32^phi + gamma_E^1 * ($N32*F32)^phi)^invPhi</f>
-        <v>2.2494521352935246</v>
+        <f t="shared" si="6"/>
+        <v>2.2498505799067563</v>
       </c>
       <c r="Q32" s="123">
-        <f>((1-gamma_E)^1 * P32^phi + gamma_E^1 * ($N32*G32)^phi)^invPhi</f>
-        <v>2.2553014933279099</v>
+        <f t="shared" si="7"/>
+        <v>2.2556582465405937</v>
       </c>
       <c r="R32" s="123"/>
     </row>
@@ -31511,7 +31515,7 @@
       </c>
       <c r="D33" s="123">
         <f>USData!D33</f>
-        <v>1.3741821007782271</v>
+        <v>1.3521966436241903</v>
       </c>
       <c r="E33" s="123">
         <f>USData!E33</f>
@@ -31529,25 +31533,25 @@
         <f>USData!H33</f>
         <v>NA</v>
       </c>
-      <c r="M33" s="152">
-        <f>EXP(lambda_L*B33)</f>
+      <c r="M33" s="138">
+        <f t="shared" si="0"/>
         <v>1.5434188681164871</v>
       </c>
-      <c r="N33" s="152">
-        <f>EXP(lambda_E*B33)</f>
+      <c r="N33" s="138">
+        <f t="shared" si="1"/>
         <v>1.947409445764859</v>
       </c>
       <c r="O33" s="123">
-        <f>E33^alpha * (M33*D33)^beta</f>
-        <v>2.3237011284659856</v>
+        <f t="shared" si="2"/>
+        <v>2.2966512396662986</v>
       </c>
       <c r="P33" s="123">
-        <f>((1-gamma_E)^1 * O33^phi + gamma_E^1 * ($N33*F33)^phi)^invPhi</f>
-        <v>2.3267584930386085</v>
+        <f t="shared" si="6"/>
+        <v>2.301680692031975</v>
       </c>
       <c r="Q33" s="123">
-        <f>((1-gamma_E)^1 * P33^phi + gamma_E^1 * ($N33*G33)^phi)^invPhi</f>
-        <v>2.3289156298921472</v>
+        <f t="shared" si="7"/>
+        <v>2.3051818817875227</v>
       </c>
       <c r="R33" s="123"/>
     </row>

</xml_diff>